<commit_message>
Commit atualização do projeto com rede de gerenciamento e dados
</commit_message>
<xml_diff>
--- a/reports/discovery_report_COMPLETO.xlsx
+++ b/reports/discovery_report_COMPLETO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.166.151</t>
+          <t>192.168.166.170</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FastEthernet0/0</t>
+          <t>FastEthernet2/0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,22 +495,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.10.4</t>
+          <t>192.168.166.172</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ethernet0/3</t>
+          <t>FastEthernet1/0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>S4.lab.local</t>
+          <t>S2.lab.local</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Linux Unix</t>
+          <t>Cisco 3725</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.166.151</t>
+          <t>192.168.166.173</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,12 +539,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Roteador-3725</t>
+          <t>S3.lab.local</t>
         </is>
       </c>
     </row>
@@ -556,22 +556,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.20.2</t>
+          <t>192.168.166.172</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ethernet0/0</t>
+          <t>FastEthernet1/1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>S6.lab.local</t>
+          <t>S2.lab.local</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Linux Unix</t>
+          <t>Cisco 3725</t>
         </is>
       </c>
     </row>
@@ -582,6 +582,67 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dispositivo Raiz</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.166.172</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FastEthernet1/2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>S2.lab.local</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Vizinho Conectado</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.166.174</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>FastEthernet1/0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>S4.lab.local</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Cisco 3725</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit resultado perfeito + salvamento do json
</commit_message>
<xml_diff>
--- a/reports/discovery_report_COMPLETO.xlsx
+++ b/reports/discovery_report_COMPLETO.xlsx
@@ -55,25 +55,25 @@
     <t>Dispositivo Principal: S6</t>
   </si>
   <si>
-    <t>192.168.166.175</t>
-  </si>
-  <si>
-    <t>192.168.166.180</t>
-  </si>
-  <si>
-    <t>192.168.166.176</t>
-  </si>
-  <si>
-    <t>192.168.166.179</t>
-  </si>
-  <si>
-    <t>192.168.166.178</t>
-  </si>
-  <si>
-    <t>192.168.166.177</t>
-  </si>
-  <si>
-    <t>192.168.166.181</t>
+    <t>192.168.166.182</t>
+  </si>
+  <si>
+    <t>192.168.166.183</t>
+  </si>
+  <si>
+    <t>192.168.166.184</t>
+  </si>
+  <si>
+    <t>192.168.166.187</t>
+  </si>
+  <si>
+    <t>192.168.166.185</t>
+  </si>
+  <si>
+    <t>192.168.166.186</t>
+  </si>
+  <si>
+    <t>192.168.166.188</t>
   </si>
   <si>
     <t>FastEthernet1/0</t>

</xml_diff>